<commit_message>
completed functional simulation screnshots and working on some documentations
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G54-4794-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G54-4794-350-1201.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Ensc_350\Assignments-350\1201\Labwork\FP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ENSC350\FP2.2-350-1201\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC6787F-6BB0-486B-95D5-E5DACEAF45A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA675607-DC61-4B1D-BB57-63CA56348D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
     <sheet name="Activity Log - Part 2" sheetId="4" r:id="rId2"/>
     <sheet name="Activity Log - Part 3" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -122,6 +124,63 @@
   </si>
   <si>
     <t>Gxx</t>
+  </si>
+  <si>
+    <t>Started reading about the implementation of Arithmetic Unit</t>
+  </si>
+  <si>
+    <t>Setting up work environment, git and modelsim</t>
+  </si>
+  <si>
+    <t>Worked on full adder implementation</t>
+  </si>
+  <si>
+    <t>Worked on ripple adder implementation</t>
+  </si>
+  <si>
+    <t>Worked on arithmetic unit implementing Adder, Zero, ExtWord MUX, AltB  and AltBu</t>
+  </si>
+  <si>
+    <t>Help debug arithmetic unit (errors with sign extension) Output ExtWord was not matching with test bench values</t>
+  </si>
+  <si>
+    <t>Screenshots of waves of functional simulation</t>
+  </si>
+  <si>
+    <t>Helping with screenshots of timing simulations</t>
+  </si>
+  <si>
+    <t>Start working on documentations, screenshot descriptions, etc.</t>
+  </si>
+  <si>
+    <t>Writing up report and proofreading</t>
+  </si>
+  <si>
+    <t>Cleaning up documentations and finishing up</t>
+  </si>
+  <si>
+    <t>Adding anotations to pdf</t>
+  </si>
+  <si>
+    <t>Added table of contents, formatting and submitting</t>
+  </si>
+  <si>
+    <t>G54</t>
+  </si>
+  <si>
+    <t>Yoel Yonata</t>
+  </si>
+  <si>
+    <t>Worked on SLL, SRL and SRA</t>
+  </si>
+  <si>
+    <t>Worked on Execution Unit</t>
+  </si>
+  <si>
+    <t>Started reading on project part 2 and how to implement</t>
+  </si>
+  <si>
+    <t>Debugging SRA, sign extension was not working</t>
   </si>
 </sst>
 </file>
@@ -229,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -426,11 +485,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -565,6 +648,27 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -920,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E6E40-83BD-4CBB-97D3-102021CD8368}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +1045,9 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="37" t="s">
+        <v>28</v>
+      </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="38" t="s">
@@ -954,7 +1060,9 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="39">
+        <v>301304794</v>
+      </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="38"/>
@@ -966,7 +1074,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -982,7 +1090,7 @@
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="41" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -1001,174 +1109,304 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="B6" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C6" s="43">
+        <v>43919</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="16"/>
+      <c r="G6" s="45" t="s">
+        <v>14</v>
+      </c>
       <c r="H6" s="12">
         <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
-        <v>0</v>
+        <v>0.50000000000000089</v>
       </c>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C7" s="43">
+        <v>43919</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.94791666666666663</v>
+      </c>
       <c r="F7" s="34"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="46" t="s">
+        <v>15</v>
+      </c>
       <c r="H7" s="27">
         <f>(E7-D7)*24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.83333333333333037</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="33"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C8" s="43">
+        <v>43920</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.90625</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="46" t="s">
+        <v>16</v>
+      </c>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.91666666666666874</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="33"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C9" s="43">
+        <v>43920</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.90625</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.95138888888888884</v>
+      </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="46" t="s">
+        <v>17</v>
+      </c>
       <c r="H9" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.0833333333333321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="33"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C10" s="43">
+        <v>43921</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.93055555555555547</v>
+      </c>
       <c r="F10" s="34"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="46" t="s">
+        <v>18</v>
+      </c>
       <c r="H10" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.6666666666666634</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="33"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="23"/>
+      <c r="B11" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C11" s="43">
+        <v>43922</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="46" t="s">
+        <v>19</v>
+      </c>
       <c r="H11" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="33"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="23"/>
+      <c r="B12" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C12" s="43">
+        <v>43923</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="F12" s="34"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="46" t="s">
+        <v>20</v>
+      </c>
       <c r="H12" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.0000000000000018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="33"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C13" s="42">
+        <v>43923</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.86458333333333337</v>
+      </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="47" t="s">
+        <v>21</v>
+      </c>
       <c r="H13" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.0833333333333321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="33"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="23"/>
+      <c r="B14" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C14" s="43">
+        <v>43923</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="E14" s="23">
+        <v>0.94791666666666663</v>
+      </c>
       <c r="F14" s="34"/>
-      <c r="G14" s="17"/>
+      <c r="G14" s="46" t="s">
+        <v>22</v>
+      </c>
       <c r="H14" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.9999999999999982</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="33"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="23"/>
+      <c r="B15" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C15" s="43">
+        <v>43924</v>
+      </c>
+      <c r="D15" s="20">
+        <v>0.71875</v>
+      </c>
+      <c r="E15" s="23">
+        <v>0.76388888888888884</v>
+      </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="46" t="s">
+        <v>23</v>
+      </c>
       <c r="H15" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.0833333333333321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="33"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C16" s="43">
+        <v>43926</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="E16" s="23">
+        <v>0.67708333333333337</v>
+      </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="46" t="s">
+        <v>24</v>
+      </c>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.5833333333333357</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="33"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C17" s="43">
+        <v>43926</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E17" s="23">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="F17" s="34"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="46" t="s">
+        <v>25</v>
+      </c>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2499999999999982</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C18" s="42">
+        <v>43926</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="E18" s="23">
+        <v>0.93055555555555547</v>
+      </c>
       <c r="F18" s="34"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="44" t="s">
+        <v>26</v>
+      </c>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0833333333333321</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1955,7 +2193,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>0</v>
+        <v>15.583333333333325</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2683,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD091BD6-3364-44DE-8BB4-985458F62AD8}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2704,7 +2942,9 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="37" t="s">
+        <v>28</v>
+      </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="38" t="s">
@@ -2717,7 +2957,9 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="39">
+        <v>301304794</v>
+      </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="38"/>
@@ -2729,7 +2971,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -2764,57 +3006,97 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="B6" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C6" s="19">
+        <v>43931</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0.92708333333333337</v>
+      </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="H6" s="12">
         <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
-        <v>0</v>
+        <v>1.0000000000000018</v>
       </c>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C7" s="19">
+        <v>43931</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.98958333333333337</v>
+      </c>
       <c r="F7" s="34"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="H7" s="27">
         <f>(E7-D7)*24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="33"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C8" s="19">
+        <v>43932</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
-        <v>0</v>
+        <v>1.0833333333333321</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C9" s="19">
+        <v>43932</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.99305555555555547</v>
+      </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="H9" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9999999999999982</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3718,7 +4000,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>0</v>
+        <v>5.5833333333333321</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4446,7 +4728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating logs, updated screenshots
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G54-4794-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G54-4794-350-1201.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ENSC350\FP2.2-350-1201\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA675607-DC61-4B1D-BB57-63CA56348D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA7814C-13AA-47E0-80D4-BE40D60DE9B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -171,16 +171,40 @@
     <t>Yoel Yonata</t>
   </si>
   <si>
-    <t>Worked on SLL, SRL and SRA</t>
-  </si>
-  <si>
-    <t>Worked on Execution Unit</t>
-  </si>
-  <si>
     <t>Started reading on project part 2 and how to implement</t>
   </si>
   <si>
-    <t>Debugging SRA, sign extension was not working</t>
+    <t>Was not able to synthesize shift unit due to resize function, changing SRA implementation</t>
+  </si>
+  <si>
+    <t>Worked on Execution Unit, should be able to test it as soon all components are working as intended</t>
+  </si>
+  <si>
+    <t>Synthesizing execution unit. No problems with the execution unit. Synthesize completed.</t>
+  </si>
+  <si>
+    <t>Debugging SRA, sign extension was not working.</t>
+  </si>
+  <si>
+    <t>Worked on SLL, SRL and SRA. A few errors in SRA will look into it. SLL and SRL is completed. Will need to be tested</t>
+  </si>
+  <si>
+    <t>Taking screenshots of all 32 bit shift functional simulation.</t>
+  </si>
+  <si>
+    <t>Performing timing simulation of 64 bit shifts. Taking screenshots</t>
+  </si>
+  <si>
+    <t>Running both functional and timing simulations of the arithmetic unit. Taking screenshots as well.</t>
+  </si>
+  <si>
+    <t>Retaking a few screenshots. Arithmetic unit timing simulation screenshots are cut off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working on documentations. Adding descriptions to each screenshots. </t>
+  </si>
+  <si>
+    <t>Most wave screenshots description are completed.  A few more descriptions needed for RTL and postfit screenshots</t>
   </si>
 </sst>
 </file>
@@ -635,21 +659,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="18" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -669,6 +678,21 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1045,42 +1069,42 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="46">
         <v>301304794</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1090,7 +1114,7 @@
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="37" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -1114,7 +1138,7 @@
       <c r="B6" s="13">
         <v>4794</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="39">
         <v>43919</v>
       </c>
       <c r="D6" s="20">
@@ -1124,7 +1148,7 @@
         <v>0.90972222222222221</v>
       </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="41" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="12">
@@ -1138,7 +1162,7 @@
       <c r="B7" s="13">
         <v>4794</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="39">
         <v>43919</v>
       </c>
       <c r="D7" s="20">
@@ -1148,7 +1172,7 @@
         <v>0.94791666666666663</v>
       </c>
       <c r="F7" s="34"/>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="42" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="27">
@@ -1161,7 +1185,7 @@
       <c r="B8" s="13">
         <v>4794</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="39">
         <v>43920</v>
       </c>
       <c r="D8" s="20">
@@ -1171,7 +1195,7 @@
         <v>0.90625</v>
       </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="42" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="27">
@@ -1184,7 +1208,7 @@
       <c r="B9" s="13">
         <v>4794</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="39">
         <v>43920</v>
       </c>
       <c r="D9" s="20">
@@ -1194,7 +1218,7 @@
         <v>0.95138888888888884</v>
       </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="42" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="27">
@@ -1207,7 +1231,7 @@
       <c r="B10" s="13">
         <v>4794</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="39">
         <v>43921</v>
       </c>
       <c r="D10" s="20">
@@ -1217,7 +1241,7 @@
         <v>0.93055555555555547</v>
       </c>
       <c r="F10" s="34"/>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="42" t="s">
         <v>18</v>
       </c>
       <c r="H10" s="27">
@@ -1230,7 +1254,7 @@
       <c r="B11" s="13">
         <v>4794</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="39">
         <v>43922</v>
       </c>
       <c r="D11" s="20">
@@ -1240,7 +1264,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="46" t="s">
+      <c r="G11" s="42" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="27">
@@ -1253,7 +1277,7 @@
       <c r="B12" s="13">
         <v>4794</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="39">
         <v>43923</v>
       </c>
       <c r="D12" s="20">
@@ -1263,7 +1287,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="F12" s="34"/>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="42" t="s">
         <v>20</v>
       </c>
       <c r="H12" s="27">
@@ -1276,7 +1300,7 @@
       <c r="B13" s="13">
         <v>4794</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="38">
         <v>43923</v>
       </c>
       <c r="D13" s="20">
@@ -1286,7 +1310,7 @@
         <v>0.86458333333333337</v>
       </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="43" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="27">
@@ -1299,7 +1323,7 @@
       <c r="B14" s="13">
         <v>4794</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="39">
         <v>43923</v>
       </c>
       <c r="D14" s="20">
@@ -1309,7 +1333,7 @@
         <v>0.94791666666666663</v>
       </c>
       <c r="F14" s="34"/>
-      <c r="G14" s="46" t="s">
+      <c r="G14" s="42" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="27">
@@ -1322,7 +1346,7 @@
       <c r="B15" s="13">
         <v>4794</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="39">
         <v>43924</v>
       </c>
       <c r="D15" s="20">
@@ -1332,7 +1356,7 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="46" t="s">
+      <c r="G15" s="42" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="27">
@@ -1345,7 +1369,7 @@
       <c r="B16" s="13">
         <v>4794</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="39">
         <v>43926</v>
       </c>
       <c r="D16" s="20">
@@ -1355,7 +1379,7 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="46" t="s">
+      <c r="G16" s="42" t="s">
         <v>24</v>
       </c>
       <c r="H16" s="27">
@@ -1368,7 +1392,7 @@
       <c r="B17" s="13">
         <v>4794</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="39">
         <v>43926</v>
       </c>
       <c r="D17" s="20">
@@ -1378,7 +1402,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="F17" s="34"/>
-      <c r="G17" s="46" t="s">
+      <c r="G17" s="42" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="27">
@@ -1391,7 +1415,7 @@
       <c r="B18" s="13">
         <v>4794</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="38">
         <v>43926</v>
       </c>
       <c r="D18" s="20">
@@ -1401,7 +1425,7 @@
         <v>0.93055555555555547</v>
       </c>
       <c r="F18" s="34"/>
-      <c r="G18" s="44" t="s">
+      <c r="G18" s="40" t="s">
         <v>26</v>
       </c>
       <c r="H18" s="27">
@@ -2922,7 +2946,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2942,42 +2966,42 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="46">
         <v>301304794</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3022,7 +3046,7 @@
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
@@ -3046,7 +3070,7 @@
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="17" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H7" s="27">
         <f>(E7-D7)*24</f>
@@ -3069,7 +3093,7 @@
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
@@ -3092,7 +3116,7 @@
       </c>
       <c r="F9" s="34"/>
       <c r="G9" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H9" s="27">
         <f t="shared" si="1"/>
@@ -3101,106 +3125,186 @@
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C10" s="22">
+        <v>43935</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.77430555555555547</v>
+      </c>
       <c r="F10" s="34"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="H10" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4999999999999991</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="23"/>
+      <c r="B11" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C11" s="22">
+        <v>43935</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="H11" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="23"/>
+      <c r="B12" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C12" s="22">
+        <v>43935</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0.88541666666666663</v>
+      </c>
       <c r="F12" s="34"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="H12" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C13" s="22">
+        <v>43935</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="H13" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="23"/>
+      <c r="B14" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C14" s="22">
+        <v>43935</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E14" s="23">
+        <v>0.9375</v>
+      </c>
       <c r="F14" s="34"/>
-      <c r="G14" s="17"/>
+      <c r="G14" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="H14" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.50000000000000089</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="23"/>
+      <c r="B15" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C15" s="22">
+        <v>43936</v>
+      </c>
+      <c r="D15" s="20">
+        <v>0.85763888888888884</v>
+      </c>
+      <c r="E15" s="23">
+        <v>0.88541666666666663</v>
+      </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="17" t="s">
+        <v>38</v>
+      </c>
       <c r="H15" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.66666666666666696</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C16" s="22">
+        <v>43936</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="E16" s="23">
+        <v>0.99652777777777779</v>
+      </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.6666666666666679</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C17" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D17" s="23">
+        <v>0</v>
+      </c>
+      <c r="E17" s="23">
+        <v>4.8611111111111112E-2</v>
+      </c>
       <c r="F17" s="34"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.1666666666666667</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4000,7 +4104,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>5.5833333333333321</v>
+        <v>15.333333333333334</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4749,38 +4853,38 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated screenshots and logs
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G54-4794-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G54-4794-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA7814C-13AA-47E0-80D4-BE40D60DE9B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEC4921-C2E3-4B7E-9F7D-5CB7FF155058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>Most wave screenshots description are completed.  A few more descriptions needed for RTL and postfit screenshots</t>
+  </si>
+  <si>
+    <t>Finishing screenshots description for RTL and postfit circuits. Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redoing some screen captures of SLL, SRL and SRA 32 Timing simulation because some info was illegible. </t>
+  </si>
+  <si>
+    <t>Proofreading all documentations and fixing errors. Fixed typos and miscalculations.</t>
+  </si>
+  <si>
+    <t>Working on annotating screenshots. Annotations mostly completed.</t>
   </si>
 </sst>
 </file>
@@ -2946,7 +2958,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3309,54 +3321,94 @@
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C18" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="E18" s="23">
+        <v>0.71875</v>
+      </c>
       <c r="F18" s="34"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0833333333333321</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="23"/>
+      <c r="B19" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C19" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0.71875</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0.78125</v>
+      </c>
       <c r="F19" s="34"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="H19" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="23"/>
+      <c r="B20" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C20" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0.78125</v>
+      </c>
+      <c r="E20" s="23">
+        <v>0.82638888888888884</v>
+      </c>
       <c r="F20" s="34"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0833333333333321</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="23"/>
+      <c r="B21" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C21" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0.94097222222222221</v>
+      </c>
       <c r="F21" s="34"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="H21" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.6666666666666661</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4104,7 +4156,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>15.333333333333334</v>
+        <v>20.666666666666664</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Logs and added final report
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G54-4794-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G54-4794-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEC4921-C2E3-4B7E-9F7D-5CB7FF155058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A19351D-1A37-44D2-A792-437D6D095EDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Working on annotating screenshots. Annotations mostly completed.</t>
+  </si>
+  <si>
+    <t>Final proofreading and formatting of project report.</t>
   </si>
 </sst>
 </file>
@@ -2958,7 +2961,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,15 +3416,25 @@
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="23"/>
+      <c r="B22" s="14">
+        <v>4794</v>
+      </c>
+      <c r="C22" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0.78125</v>
+      </c>
       <c r="F22" s="34"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="H22" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.166666666666667</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4156,7 +4169,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>20.666666666666664</v>
+        <v>22.833333333333332</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>